<commit_message>
Import and merge previous year registrations
</commit_message>
<xml_diff>
--- a/test/fixture/import_1.xlsx
+++ b/test/fixture/import_1.xlsx
@@ -580,7 +580,7 @@
   <dimension ref="A1:W6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -793,9 +793,6 @@
       <c r="I5" s="2">
         <v>2011</v>
       </c>
-      <c r="J5" s="2">
-        <v>2011</v>
-      </c>
       <c r="K5" s="2">
         <v>1989</v>
       </c>
@@ -832,7 +829,7 @@
         <v>2012</v>
       </c>
       <c r="J6" s="2">
-        <v>2012</v>
+        <v>2011</v>
       </c>
       <c r="K6" s="2">
         <v>1970</v>

</xml_diff>